<commit_message>
fix file for tutorial?
</commit_message>
<xml_diff>
--- a/tableau-cotton-exports.xlsx
+++ b/tableau-cotton-exports.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary Reddick\Desktop\Tutorial-Folder\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="3480" yWindow="620" windowWidth="12260" windowHeight="14160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="18">
   <si>
     <t>Month</t>
   </si>
@@ -76,15 +74,34 @@
   <si>
     <t>Great Britain</t>
   </si>
+  <si>
+    <t>Portugal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,15 +124,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -174,7 +199,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -226,7 +251,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -420,7 +445,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -428,19 +453,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X169"/>
+  <dimension ref="A1:X170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B156" sqref="B156"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C171" sqref="C171"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,18 +477,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="A2" s="2">
         <v>1828</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C2" s="1">
+        <v>78541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" s="2">
         <v>1828</v>
       </c>
@@ -470,11 +496,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f ca="1">+C3:CC43</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+        <v>4997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" s="2">
         <v>1828</v>
       </c>
@@ -482,10 +507,10 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+        <v>5499</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" s="2">
         <v>1828</v>
       </c>
@@ -493,10 +518,10 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+        <v>4353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" s="2">
         <v>1828</v>
       </c>
@@ -504,10 +529,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+        <v>3287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" s="2">
         <v>1828</v>
       </c>
@@ -515,10 +540,10 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+        <v>9656</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" s="2">
         <v>1828</v>
       </c>
@@ -526,10 +551,10 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" s="2">
         <v>1828</v>
       </c>
@@ -537,10 +562,10 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+        <v>6627</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" s="2">
         <v>1828</v>
       </c>
@@ -548,10 +573,10 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" s="2">
         <v>1828</v>
       </c>
@@ -559,10 +584,10 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12" s="2">
         <v>1828</v>
       </c>
@@ -570,10 +595,10 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13" s="2">
         <v>1828</v>
       </c>
@@ -581,10 +606,10 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14" s="2">
         <v>1828</v>
       </c>
@@ -592,11 +617,11 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="X14" s="2"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24">
       <c r="A15" s="2">
         <v>1828</v>
       </c>
@@ -606,8 +631,9 @@
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16" s="2">
         <v>1859</v>
       </c>
@@ -618,7 +644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="2">
         <v>1859</v>
       </c>
@@ -629,7 +655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="2">
         <v>1859</v>
       </c>
@@ -640,7 +666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="2">
         <v>1859</v>
       </c>
@@ -651,7 +677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="2">
         <v>1859</v>
       </c>
@@ -662,7 +688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="2">
         <v>1859</v>
       </c>
@@ -673,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="2">
         <v>1859</v>
       </c>
@@ -684,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="2">
         <v>1859</v>
       </c>
@@ -695,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="2">
         <v>1859</v>
       </c>
@@ -706,7 +732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="2">
         <v>1859</v>
       </c>
@@ -717,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="2">
         <v>1859</v>
       </c>
@@ -728,7 +754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="2">
         <v>1859</v>
       </c>
@@ -739,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="2">
         <v>1859</v>
       </c>
@@ -750,7 +776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="2">
         <v>1859</v>
       </c>
@@ -761,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="2">
         <v>1887</v>
       </c>
@@ -772,7 +798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="2">
         <v>1887</v>
       </c>
@@ -783,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="2">
         <v>1887</v>
       </c>
@@ -794,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="2">
         <v>1887</v>
       </c>
@@ -805,7 +831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="2">
         <v>1887</v>
       </c>
@@ -816,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="2">
         <v>1887</v>
       </c>
@@ -827,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="2">
         <v>1887</v>
       </c>
@@ -838,7 +864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="2">
         <v>1887</v>
       </c>
@@ -849,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="2">
         <v>1887</v>
       </c>
@@ -860,7 +886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="2">
         <v>1887</v>
       </c>
@@ -871,7 +897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="2">
         <v>1887</v>
       </c>
@@ -882,7 +908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="2">
         <v>1887</v>
       </c>
@@ -893,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="2">
         <v>1887</v>
       </c>
@@ -904,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="2">
         <v>1887</v>
       </c>
@@ -915,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="2">
         <v>1918</v>
       </c>
@@ -926,7 +952,7 @@
         <v>34109</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="2">
         <v>1918</v>
       </c>
@@ -937,7 +963,7 @@
         <v>4789</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="2">
         <v>1918</v>
       </c>
@@ -948,7 +974,7 @@
         <v>4857</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="2">
         <v>1918</v>
       </c>
@@ -959,7 +985,7 @@
         <v>3376</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="2">
         <v>1918</v>
       </c>
@@ -970,7 +996,7 @@
         <v>1777</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" s="2">
         <v>1918</v>
       </c>
@@ -981,7 +1007,7 @@
         <v>4655</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="2">
         <v>1918</v>
       </c>
@@ -992,7 +1018,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" s="2">
         <v>1918</v>
       </c>
@@ -1003,7 +1029,7 @@
         <v>3186</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="2">
         <v>1918</v>
       </c>
@@ -1014,7 +1040,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" s="2">
         <v>1918</v>
       </c>
@@ -1025,7 +1051,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" s="2">
         <v>1918</v>
       </c>
@@ -1036,7 +1062,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" s="2">
         <v>1918</v>
       </c>
@@ -1047,7 +1073,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" s="2">
         <v>1918</v>
       </c>
@@ -1058,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" s="2">
         <v>1918</v>
       </c>
@@ -1069,7 +1095,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" s="2">
         <v>1948</v>
       </c>
@@ -1080,7 +1106,7 @@
         <v>13166</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" s="2">
         <v>1948</v>
       </c>
@@ -1091,7 +1117,7 @@
         <v>4958</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" s="2">
         <v>1948</v>
       </c>
@@ -1102,7 +1128,7 @@
         <v>6456</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" s="2">
         <v>1948</v>
       </c>
@@ -1113,7 +1139,7 @@
         <v>2446</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" s="2">
         <v>1948</v>
       </c>
@@ -1124,7 +1150,7 @@
         <v>2427</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" s="2">
         <v>1948</v>
       </c>
@@ -1135,7 +1161,7 @@
         <v>5906</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" s="2">
         <v>1948</v>
       </c>
@@ -1146,7 +1172,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" s="2">
         <v>1948</v>
       </c>
@@ -1157,7 +1183,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" s="2">
         <v>1948</v>
       </c>
@@ -1168,7 +1194,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" s="2">
         <v>1948</v>
       </c>
@@ -1179,7 +1205,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" s="2">
         <v>1948</v>
       </c>
@@ -1190,7 +1216,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" s="2">
         <v>1948</v>
       </c>
@@ -1201,7 +1227,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" s="2">
         <v>1948</v>
       </c>
@@ -1212,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" s="2">
         <v>1948</v>
       </c>
@@ -1223,7 +1249,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" s="2">
         <v>1979</v>
       </c>
@@ -1234,7 +1260,7 @@
         <v>24103</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" s="2">
         <v>1979</v>
       </c>
@@ -1245,7 +1271,7 @@
         <v>7733</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" s="2">
         <v>1979</v>
       </c>
@@ -1256,7 +1282,7 @@
         <v>2851</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" s="2">
         <v>1979</v>
       </c>
@@ -1267,7 +1293,7 @@
         <v>4187</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" s="2">
         <v>1979</v>
       </c>
@@ -1278,7 +1304,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" s="2">
         <v>1979</v>
       </c>
@@ -1289,7 +1315,7 @@
         <v>6217</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" s="2">
         <v>1979</v>
       </c>
@@ -1300,7 +1326,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" s="2">
         <v>1979</v>
       </c>
@@ -1311,7 +1337,7 @@
         <v>2429</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" s="2">
         <v>1979</v>
       </c>
@@ -1322,7 +1348,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" s="2">
         <v>1979</v>
       </c>
@@ -1333,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" s="2">
         <v>1979</v>
       </c>
@@ -1344,7 +1370,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" s="2">
         <v>1979</v>
       </c>
@@ -1355,7 +1381,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" s="2">
         <v>1979</v>
       </c>
@@ -1366,7 +1392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" s="2">
         <v>1979</v>
       </c>
@@ -1377,7 +1403,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86" s="2">
         <v>2009</v>
       </c>
@@ -1388,7 +1414,7 @@
         <v>25231</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" s="2">
         <v>2009</v>
       </c>
@@ -1399,7 +1425,7 @@
         <v>4492</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" s="2">
         <v>2009</v>
       </c>
@@ -1410,7 +1436,7 @@
         <v>4606</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" s="2">
         <v>2009</v>
       </c>
@@ -1421,7 +1447,7 @@
         <v>2718</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3">
       <c r="A90" s="2">
         <v>2009</v>
       </c>
@@ -1432,7 +1458,7 @@
         <v>1718</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91" s="2">
         <v>2009</v>
       </c>
@@ -1443,7 +1469,7 @@
         <v>4427</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="A92" s="2">
         <v>2009</v>
       </c>
@@ -1454,7 +1480,7 @@
         <v>1659</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="A93" s="2">
         <v>2009</v>
       </c>
@@ -1465,7 +1491,7 @@
         <v>2663</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="A94" s="2">
         <v>2009</v>
       </c>
@@ -1476,7 +1502,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="A95" s="2">
         <v>2009</v>
       </c>
@@ -1487,7 +1513,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96" s="2">
         <v>2009</v>
       </c>
@@ -1498,7 +1524,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3">
       <c r="A97" s="2">
         <v>2009</v>
       </c>
@@ -1509,7 +1535,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3">
       <c r="A98" s="2">
         <v>2009</v>
       </c>
@@ -1520,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3">
       <c r="A99" s="2">
         <v>2009</v>
       </c>
@@ -1531,7 +1557,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3">
       <c r="A100" s="2">
         <v>2040</v>
       </c>
@@ -1539,10 +1565,10 @@
         <v>16</v>
       </c>
       <c r="C100" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20495</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" s="2">
         <v>2040</v>
       </c>
@@ -1550,10 +1576,10 @@
         <v>1</v>
       </c>
       <c r="C101" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3547</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" s="2">
         <v>2040</v>
       </c>
@@ -1561,10 +1587,10 @@
         <v>2</v>
       </c>
       <c r="C102" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4490</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" s="2">
         <v>2040</v>
       </c>
@@ -1572,10 +1598,10 @@
         <v>3</v>
       </c>
       <c r="C103" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" s="2">
         <v>2040</v>
       </c>
@@ -1583,10 +1609,10 @@
         <v>4</v>
       </c>
       <c r="C104" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" s="2">
         <v>2040</v>
       </c>
@@ -1594,10 +1620,10 @@
         <v>10</v>
       </c>
       <c r="C105" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5083</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" s="2">
         <v>2040</v>
       </c>
@@ -1605,10 +1631,10 @@
         <v>5</v>
       </c>
       <c r="C106" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" s="2">
         <v>2040</v>
       </c>
@@ -1616,10 +1642,10 @@
         <v>11</v>
       </c>
       <c r="C107" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2417</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108" s="2">
         <v>2040</v>
       </c>
@@ -1627,10 +1653,10 @@
         <v>6</v>
       </c>
       <c r="C108" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109" s="2">
         <v>2040</v>
       </c>
@@ -1641,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3">
       <c r="A110" s="2">
         <v>2040</v>
       </c>
@@ -1649,10 +1675,10 @@
         <v>8</v>
       </c>
       <c r="C110" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
       <c r="A111" s="2">
         <v>2040</v>
       </c>
@@ -1660,10 +1686,10 @@
         <v>9</v>
       </c>
       <c r="C111" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
       <c r="A112" s="2">
         <v>2040</v>
       </c>
@@ -1674,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3">
       <c r="A113" s="2">
         <v>2040</v>
       </c>
@@ -1682,10 +1708,10 @@
         <v>14</v>
       </c>
       <c r="C113" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" s="2">
         <v>2071</v>
       </c>
@@ -1696,7 +1722,7 @@
         <v>18784</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3">
       <c r="A115" s="2">
         <v>2071</v>
       </c>
@@ -1707,7 +1733,7 @@
         <v>2733</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3">
       <c r="A116" s="2">
         <v>2071</v>
       </c>
@@ -1718,7 +1744,7 @@
         <v>2746</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3">
       <c r="A117" s="2">
         <v>2071</v>
       </c>
@@ -1729,7 +1755,7 @@
         <v>2124</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3">
       <c r="A118" s="2">
         <v>2071</v>
       </c>
@@ -1740,7 +1766,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3">
       <c r="A119" s="2">
         <v>2071</v>
       </c>
@@ -1751,7 +1777,7 @@
         <v>8428</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3">
       <c r="A120" s="2">
         <v>2071</v>
       </c>
@@ -1762,7 +1788,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3">
       <c r="A121" s="2">
         <v>2071</v>
       </c>
@@ -1773,7 +1799,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3">
       <c r="A122" s="2">
         <v>2071</v>
       </c>
@@ -1784,7 +1810,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3">
       <c r="A123" s="2">
         <v>2071</v>
       </c>
@@ -1795,7 +1821,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3">
       <c r="A124" s="2">
         <v>2071</v>
       </c>
@@ -1806,7 +1832,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3">
       <c r="A125" s="2">
         <v>2071</v>
       </c>
@@ -1817,7 +1843,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3">
       <c r="A126" s="2">
         <v>2071</v>
       </c>
@@ -1828,7 +1854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3">
       <c r="A127" s="2">
         <v>2071</v>
       </c>
@@ -1839,7 +1865,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3">
       <c r="A128" s="2">
         <v>2101</v>
       </c>
@@ -1847,10 +1873,10 @@
         <v>16</v>
       </c>
       <c r="C128" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52881</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" s="2">
         <v>2101</v>
       </c>
@@ -1858,10 +1884,10 @@
         <v>1</v>
       </c>
       <c r="C129" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6366</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" s="2">
         <v>2101</v>
       </c>
@@ -1869,10 +1895,10 @@
         <v>2</v>
       </c>
       <c r="C130" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4367</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" s="2">
         <v>2101</v>
       </c>
@@ -1880,10 +1906,10 @@
         <v>3</v>
       </c>
       <c r="C131" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" s="2">
         <v>2101</v>
       </c>
@@ -1891,10 +1917,10 @@
         <v>4</v>
       </c>
       <c r="C132" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2599</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" s="2">
         <v>2101</v>
       </c>
@@ -1902,10 +1928,10 @@
         <v>10</v>
       </c>
       <c r="C133" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4782</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" s="2">
         <v>2101</v>
       </c>
@@ -1913,10 +1939,10 @@
         <v>5</v>
       </c>
       <c r="C134" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" s="2">
         <v>2101</v>
       </c>
@@ -1924,10 +1950,10 @@
         <v>11</v>
       </c>
       <c r="C135" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3294</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="2">
         <v>2101</v>
       </c>
@@ -1935,10 +1961,10 @@
         <v>6</v>
       </c>
       <c r="C136" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" s="2">
         <v>2101</v>
       </c>
@@ -1946,10 +1972,10 @@
         <v>7</v>
       </c>
       <c r="C137" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" s="2">
         <v>2101</v>
       </c>
@@ -1960,7 +1986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4">
       <c r="A139" s="2">
         <v>2101</v>
       </c>
@@ -1968,10 +1994,10 @@
         <v>9</v>
       </c>
       <c r="C139" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" s="2">
         <v>2101</v>
       </c>
@@ -1982,7 +2008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4">
       <c r="A141" s="2">
         <v>2101</v>
       </c>
@@ -1990,10 +2016,11 @@
         <v>14</v>
       </c>
       <c r="C141" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="D141" s="1"/>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" s="2">
         <v>2132</v>
       </c>
@@ -2001,10 +2028,10 @@
         <v>16</v>
       </c>
       <c r="C142" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+        <v>80123</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" s="2">
         <v>2132</v>
       </c>
@@ -2012,10 +2039,10 @@
         <v>1</v>
       </c>
       <c r="C143" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9922</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" s="2">
         <v>2132</v>
       </c>
@@ -2023,10 +2050,10 @@
         <v>2</v>
       </c>
       <c r="C144" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6667</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" s="2">
         <v>2132</v>
       </c>
@@ -2034,10 +2061,10 @@
         <v>3</v>
       </c>
       <c r="C145" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4498</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" s="2">
         <v>2132</v>
       </c>
@@ -2045,10 +2072,10 @@
         <v>4</v>
       </c>
       <c r="C146" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5593</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" s="2">
         <v>2132</v>
       </c>
@@ -2056,10 +2083,10 @@
         <v>10</v>
       </c>
       <c r="C147" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7145</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" s="2">
         <v>2132</v>
       </c>
@@ -2067,10 +2094,10 @@
         <v>5</v>
       </c>
       <c r="C148" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2092</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149" s="2">
         <v>2132</v>
       </c>
@@ -2078,10 +2105,10 @@
         <v>11</v>
       </c>
       <c r="C149" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5857</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150" s="2">
         <v>2132</v>
       </c>
@@ -2089,10 +2116,10 @@
         <v>6</v>
       </c>
       <c r="C150" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" s="2">
         <v>2132</v>
       </c>
@@ -2100,10 +2127,10 @@
         <v>7</v>
       </c>
       <c r="C151" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
       <c r="A152" s="2">
         <v>2132</v>
       </c>
@@ -2111,10 +2138,10 @@
         <v>8</v>
       </c>
       <c r="C152" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
       <c r="A153" s="2">
         <v>2132</v>
       </c>
@@ -2122,10 +2149,10 @@
         <v>9</v>
       </c>
       <c r="C153" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154" s="2">
         <v>2132</v>
       </c>
@@ -2133,10 +2160,10 @@
         <v>12</v>
       </c>
       <c r="C154" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
       <c r="A155" s="2">
         <v>2132</v>
       </c>
@@ -2144,164 +2171,182 @@
         <v>14</v>
       </c>
       <c r="C155" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>2162</v>
+        <v>2132</v>
       </c>
       <c r="B156" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C156" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="D156" s="1"/>
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157" s="2">
         <v>2162</v>
       </c>
       <c r="B157" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C157" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68182</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" s="2">
         <v>2162</v>
       </c>
       <c r="B158" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C158" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8654</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
       <c r="A159" s="2">
         <v>2162</v>
       </c>
       <c r="B159" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C159" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5030</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
       <c r="A160" s="2">
         <v>2162</v>
       </c>
       <c r="B160" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C160" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5032</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
       <c r="A161" s="2">
         <v>2162</v>
       </c>
       <c r="B161" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C161" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6034</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
       <c r="A162" s="2">
         <v>2162</v>
       </c>
       <c r="B162" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C162" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8970</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
       <c r="A163" s="2">
         <v>2162</v>
       </c>
       <c r="B163" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C163" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2870</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
       <c r="A164" s="2">
         <v>2162</v>
       </c>
       <c r="B164" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C164" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6055</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
       <c r="A165" s="2">
         <v>2162</v>
       </c>
       <c r="B165" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C165" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
       <c r="A166" s="2">
         <v>2162</v>
       </c>
       <c r="B166" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C166" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
       <c r="A167" s="2">
         <v>2162</v>
       </c>
       <c r="B167" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C167" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
       <c r="A168" s="2">
         <v>2162</v>
       </c>
       <c r="B168" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C168" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
       <c r="A169" s="2">
         <v>2162</v>
       </c>
       <c r="B169" t="s">
+        <v>12</v>
+      </c>
+      <c r="C169" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="2">
+        <v>2162</v>
+      </c>
+      <c r="B170" t="s">
         <v>14</v>
       </c>
-      <c r="C169" s="1">
-        <v>0</v>
+      <c r="C170" s="1">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>